<commit_message>
updated pcb fabrication files
</commit_message>
<xml_diff>
--- a/gerber/BOM.xlsx
+++ b/gerber/BOM.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="BOM_v2.1.4_PCB-v2.1.4_2024-06-0" state="visible" r:id="rId4"/>
+    <sheet sheetId="1" name="BOM_v2.1.4_1_PCB-v2.1.4_1_2024-" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="149">
   <si>
     <t>No.</t>
   </si>
@@ -166,7 +166,7 @@
     <t>7</t>
   </si>
   <si>
-    <t>X4621WVS-2X04I-C40D64</t>
+    <t>Molex 87759-7648</t>
   </si>
   <si>
     <t>H1</t>
@@ -175,289 +175,280 @@
     <t>HDR-SMD_8P-P2.00-V-M-R2-C4-S2.0</t>
   </si>
   <si>
-    <t>X4621WVS-2x04I-C40D64</t>
+    <t>87759-7648</t>
+  </si>
+  <si>
+    <t>Molex</t>
+  </si>
+  <si>
+    <t>538-87759-7648</t>
+  </si>
+  <si>
+    <t>Mouser</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>HLK-LD2410B-P</t>
+  </si>
+  <si>
+    <t>LD2410</t>
+  </si>
+  <si>
+    <t>newld2410</t>
+  </si>
+  <si>
+    <t>HI-LINK(海凌科)</t>
+  </si>
+  <si>
+    <t>C5183132</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>Header-Male-2.54_1x6</t>
+  </si>
+  <si>
+    <t>PROG-ESP32</t>
+  </si>
+  <si>
+    <t>hdr-th_6p-p2.54-v-m-1</t>
+  </si>
+  <si>
+    <t>2.54-1x6P直针</t>
+  </si>
+  <si>
+    <t>BOOMELE(博穆精密)</t>
+  </si>
+  <si>
+    <t>C37208</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>FDN304P</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>SOT-23-3_L2.9-W1.6-P1.90-LS2.8-BR</t>
+  </si>
+  <si>
+    <t>onsemi(安森美)</t>
+  </si>
+  <si>
+    <t>C241803</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>FDV305N</t>
+  </si>
+  <si>
+    <t>Q6,Q7</t>
+  </si>
+  <si>
+    <t>SOT-23-3_L2.9-W1.3-P1.90-LS2.4-BR</t>
+  </si>
+  <si>
+    <t>C154511</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>10kΩ</t>
+  </si>
+  <si>
+    <t>R1,R4,R5,R8,R9,R12,R17,R20</t>
+  </si>
+  <si>
+    <t>R0603</t>
+  </si>
+  <si>
+    <t>TC0325D1002T5E</t>
+  </si>
+  <si>
+    <t>UNI-ROYAL(厚声)</t>
+  </si>
+  <si>
+    <t>C425463</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>100kΩ</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>TC0325D1003T5E</t>
+  </si>
+  <si>
+    <t>C415143</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>100Ω</t>
+  </si>
+  <si>
+    <t>R7,R18</t>
+  </si>
+  <si>
+    <t>TC0325D1000T5E</t>
+  </si>
+  <si>
+    <t>C25201</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>120Ω</t>
+  </si>
+  <si>
+    <t>R15</t>
+  </si>
+  <si>
+    <t>0603WAJ0121T5E</t>
+  </si>
+  <si>
+    <t>C25205</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>470Ω</t>
+  </si>
+  <si>
+    <t>R16</t>
+  </si>
+  <si>
+    <t>0603WAF4700T5E</t>
+  </si>
+  <si>
+    <t>C23179</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>TS-1101-C-W</t>
+  </si>
+  <si>
+    <t>SW1,SW2</t>
+  </si>
+  <si>
+    <t>SW-SMD_L6.0-W3.3-LS8.0</t>
   </si>
   <si>
     <t>XKB Connectivity(中国星坤)</t>
   </si>
   <si>
-    <t>C917609</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>HLK-LD2410B-P</t>
-  </si>
-  <si>
-    <t>LD2410</t>
-  </si>
-  <si>
-    <t>newld2410</t>
-  </si>
-  <si>
-    <t>HI-LINK(海凌科)</t>
-  </si>
-  <si>
-    <t>C5183132</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>Header-Male-2.54_1x6</t>
-  </si>
-  <si>
-    <t>PROG-ESP32</t>
-  </si>
-  <si>
-    <t>hdr-th_6p-p2.54-v-m-1</t>
-  </si>
-  <si>
-    <t>2.54-1x6P直针</t>
-  </si>
-  <si>
-    <t>BOOMELE(博穆精密)</t>
-  </si>
-  <si>
-    <t>C37208</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>FDN304P</t>
-  </si>
-  <si>
-    <t>Q1</t>
-  </si>
-  <si>
-    <t>SOT-23-3_L2.9-W1.6-P1.90-LS2.8-BR</t>
-  </si>
-  <si>
-    <t>onsemi(安森美)</t>
-  </si>
-  <si>
-    <t>C241803</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>FDV305N</t>
-  </si>
-  <si>
-    <t>Q6,Q7</t>
-  </si>
-  <si>
-    <t>SOT-23-3_L2.9-W1.3-P1.90-LS2.4-BR</t>
-  </si>
-  <si>
-    <t>C154511</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>10kΩ</t>
-  </si>
-  <si>
-    <t>R1,R4,R5,R8,R9,R10,R12,R17</t>
-  </si>
-  <si>
-    <t>R0603</t>
-  </si>
-  <si>
-    <t>TC0325D1002T5E</t>
-  </si>
-  <si>
-    <t>UNI-ROYAL(厚声)</t>
-  </si>
-  <si>
-    <t>C425463</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>100kΩ</t>
-  </si>
-  <si>
-    <t>R3</t>
-  </si>
-  <si>
-    <t>TC0325D1003T5E</t>
-  </si>
-  <si>
-    <t>C415143</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>100Ω</t>
-  </si>
-  <si>
-    <t>R7,R18</t>
-  </si>
-  <si>
-    <t>TC0325D1000T5E</t>
-  </si>
-  <si>
-    <t>C25201</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>120Ω</t>
-  </si>
-  <si>
-    <t>R15</t>
-  </si>
-  <si>
-    <t>0603WAJ0121T5E</t>
-  </si>
-  <si>
-    <t>C25205</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>470Ω</t>
-  </si>
-  <si>
-    <t>R16</t>
-  </si>
-  <si>
-    <t>0603WAF4700T5E</t>
-  </si>
-  <si>
-    <t>C23179</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>20kΩ</t>
-  </si>
-  <si>
-    <t>R19</t>
-  </si>
-  <si>
-    <t>0603WAF2002T5E</t>
-  </si>
-  <si>
-    <t>C4184</t>
+    <t>C318938</t>
   </si>
   <si>
     <t>18</t>
   </si>
   <si>
-    <t>TS-1101-C-W</t>
-  </si>
-  <si>
-    <t>SW1,SW2</t>
-  </si>
-  <si>
-    <t>SW-SMD_L6.0-W3.3-LS8.0</t>
-  </si>
-  <si>
-    <t>C318938</t>
+    <t>MF52</t>
+  </si>
+  <si>
+    <t>THERMISTOR</t>
+  </si>
+  <si>
+    <t>RES-TH_L2.5-W2.5-P1.70-D0.3</t>
+  </si>
+  <si>
+    <t>MF52A103F3950 (A1)</t>
+  </si>
+  <si>
+    <t>时恒</t>
+  </si>
+  <si>
+    <t>C13879</t>
   </si>
   <si>
     <t>19</t>
   </si>
   <si>
-    <t>MF52</t>
-  </si>
-  <si>
-    <t>THERMISTOR</t>
-  </si>
-  <si>
-    <t>RES-TH_L2.5-W2.5-P1.70-D0.3</t>
-  </si>
-  <si>
-    <t>MF52A103F3950 (A1)</t>
-  </si>
-  <si>
-    <t>时恒</t>
-  </si>
-  <si>
-    <t>C13879</t>
+    <t>BL8071CLATR33</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>SOT-223-3_L6.5-W3.4-P2.30-LS7.0-BR</t>
+  </si>
+  <si>
+    <t>BL(上海贝岭)</t>
+  </si>
+  <si>
+    <t>C401677</t>
   </si>
   <si>
     <t>20</t>
   </si>
   <si>
-    <t>BL8071CLATR33</t>
-  </si>
-  <si>
-    <t>U4</t>
-  </si>
-  <si>
-    <t>SOT-223-3_L6.5-W3.4-P2.30-LS7.0-BR</t>
-  </si>
-  <si>
-    <t>BL(上海贝岭)</t>
-  </si>
-  <si>
-    <t>C401677</t>
+    <t>ICS-43434</t>
+  </si>
+  <si>
+    <t>U7</t>
+  </si>
+  <si>
+    <t>ics-43434</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>C9900000518</t>
   </si>
   <si>
     <t>21</t>
   </si>
   <si>
-    <t>ICS-43434</t>
-  </si>
-  <si>
-    <t>U7</t>
-  </si>
-  <si>
-    <t>ics-43434</t>
-  </si>
-  <si>
-    <t>null</t>
-  </si>
-  <si>
-    <t>C9900000518</t>
+    <t>ESP32-S3-WROOM-1-N16R8</t>
+  </si>
+  <si>
+    <t>U8</t>
+  </si>
+  <si>
+    <t>wirelm-smd_esp32-s3-wroom-1</t>
+  </si>
+  <si>
+    <t>ESPRESSIF(乐鑫)</t>
+  </si>
+  <si>
+    <t>C2913202</t>
   </si>
   <si>
     <t>22</t>
   </si>
   <si>
-    <t>ESP32-S3-WROOM-1-N16R8</t>
-  </si>
-  <si>
-    <t>U8</t>
-  </si>
-  <si>
-    <t>wirelm-smd_esp32-s3-wroom-1</t>
-  </si>
-  <si>
-    <t>ESPRESSIF(乐鑫)</t>
-  </si>
-  <si>
-    <t>C2913202</t>
+    <t>S8050</t>
+  </si>
+  <si>
+    <t>U9</t>
+  </si>
+  <si>
+    <t>KUU</t>
+  </si>
+  <si>
+    <t>C7603172</t>
   </si>
   <si>
     <t>23</t>
-  </si>
-  <si>
-    <t>S8050</t>
-  </si>
-  <si>
-    <t>U9</t>
-  </si>
-  <si>
-    <t>KUU</t>
-  </si>
-  <si>
-    <t>C7603172</t>
-  </si>
-  <si>
-    <t>24</t>
   </si>
   <si>
     <t>bc075-10-a-l-a</t>
@@ -843,7 +834,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100"/>
   </sheetViews>
@@ -1105,36 +1096,36 @@
         <v>56</v>
       </c>
       <c r="J8" t="s">
-        <v>18</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" t="s">
         <v>59</v>
       </c>
-      <c r="E9" t="s">
-        <v>60</v>
-      </c>
-      <c r="F9" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" t="s">
-        <v>58</v>
-      </c>
       <c r="H9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I9" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="J9" t="s">
         <v>18</v>
@@ -1142,31 +1133,31 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F10" t="s">
         <v>14</v>
       </c>
       <c r="G10" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H10" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I10" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="J10" t="s">
         <v>18</v>
@@ -1174,31 +1165,31 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D11" t="s">
+        <v>73</v>
+      </c>
+      <c r="E11" t="s">
+        <v>74</v>
+      </c>
+      <c r="F11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" t="s">
         <v>72</v>
       </c>
-      <c r="E11" t="s">
-        <v>73</v>
-      </c>
-      <c r="F11" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11" t="s">
-        <v>71</v>
-      </c>
       <c r="H11" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="I11" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="J11" t="s">
         <v>18</v>
@@ -1206,31 +1197,31 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B12" t="s">
         <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D12" t="s">
+        <v>79</v>
+      </c>
+      <c r="E12" t="s">
+        <v>80</v>
+      </c>
+      <c r="F12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" t="s">
         <v>78</v>
       </c>
-      <c r="E12" t="s">
-        <v>79</v>
-      </c>
-      <c r="F12" t="s">
-        <v>14</v>
-      </c>
-      <c r="G12" t="s">
-        <v>77</v>
-      </c>
       <c r="H12" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="I12" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J12" t="s">
         <v>18</v>
@@ -1238,31 +1229,31 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B13" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C13" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D13" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E13" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F13" t="s">
         <v>14</v>
       </c>
       <c r="G13" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H13" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I13" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J13" t="s">
         <v>18</v>
@@ -1270,31 +1261,31 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D14" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E14" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F14" t="s">
         <v>14</v>
       </c>
       <c r="G14" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H14" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I14" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="J14" t="s">
         <v>18</v>
@@ -1302,31 +1293,31 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B15" t="s">
         <v>19</v>
       </c>
       <c r="C15" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D15" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E15" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F15" t="s">
         <v>14</v>
       </c>
       <c r="G15" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H15" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I15" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="J15" t="s">
         <v>18</v>
@@ -1334,31 +1325,31 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B16" t="s">
         <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D16" t="s">
+        <v>101</v>
+      </c>
+      <c r="E16" t="s">
+        <v>85</v>
+      </c>
+      <c r="F16" t="s">
         <v>100</v>
       </c>
-      <c r="E16" t="s">
-        <v>84</v>
-      </c>
-      <c r="F16" t="s">
-        <v>99</v>
-      </c>
       <c r="G16" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H16" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I16" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="J16" t="s">
         <v>18</v>
@@ -1366,31 +1357,31 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B17" t="s">
         <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D17" t="s">
+        <v>106</v>
+      </c>
+      <c r="E17" t="s">
+        <v>85</v>
+      </c>
+      <c r="F17" t="s">
         <v>105</v>
       </c>
-      <c r="E17" t="s">
-        <v>84</v>
-      </c>
-      <c r="F17" t="s">
-        <v>104</v>
-      </c>
       <c r="G17" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H17" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I17" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="J17" t="s">
         <v>18</v>
@@ -1398,31 +1389,31 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B18" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="C18" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D18" t="s">
+        <v>111</v>
+      </c>
+      <c r="E18" t="s">
+        <v>112</v>
+      </c>
+      <c r="F18" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" t="s">
         <v>110</v>
       </c>
-      <c r="E18" t="s">
-        <v>84</v>
-      </c>
-      <c r="F18" t="s">
-        <v>109</v>
-      </c>
-      <c r="G18" t="s">
-        <v>111</v>
-      </c>
       <c r="H18" t="s">
-        <v>86</v>
+        <v>113</v>
       </c>
       <c r="I18" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="J18" t="s">
         <v>18</v>
@@ -1430,31 +1421,31 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D19" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="E19" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="F19" t="s">
         <v>14</v>
       </c>
       <c r="G19" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="H19" t="s">
-        <v>55</v>
+        <v>120</v>
       </c>
       <c r="I19" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="J19" t="s">
         <v>18</v>
@@ -1462,31 +1453,31 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="B20" t="s">
         <v>10</v>
       </c>
       <c r="C20" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="D20" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="E20" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="F20" t="s">
         <v>14</v>
       </c>
       <c r="G20" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H20" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="I20" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="J20" t="s">
         <v>18</v>
@@ -1494,31 +1485,31 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="B21" t="s">
         <v>10</v>
       </c>
       <c r="C21" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="D21" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="E21" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="F21" t="s">
         <v>14</v>
       </c>
       <c r="G21" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="H21" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="I21" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="J21" t="s">
         <v>18</v>
@@ -1526,31 +1517,31 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B22" t="s">
         <v>10</v>
       </c>
       <c r="C22" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="D22" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="E22" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="F22" t="s">
         <v>14</v>
       </c>
       <c r="G22" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="H22" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="I22" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="J22" t="s">
         <v>18</v>
@@ -1558,31 +1549,31 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B23" t="s">
         <v>10</v>
       </c>
       <c r="C23" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D23" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="E23" t="s">
-        <v>140</v>
+        <v>74</v>
       </c>
       <c r="F23" t="s">
         <v>14</v>
       </c>
       <c r="G23" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="H23" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="I23" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="J23" t="s">
         <v>18</v>
@@ -1590,70 +1581,38 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B24" t="s">
         <v>10</v>
       </c>
       <c r="C24" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D24" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E24" t="s">
-        <v>73</v>
+        <v>148</v>
       </c>
       <c r="F24" t="s">
         <v>14</v>
       </c>
       <c r="G24" t="s">
-        <v>144</v>
+        <v>14</v>
       </c>
       <c r="H24" t="s">
-        <v>146</v>
+        <v>14</v>
       </c>
       <c r="I24" t="s">
-        <v>147</v>
+        <v>14</v>
       </c>
       <c r="J24" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>148</v>
-      </c>
-      <c r="B25" t="s">
-        <v>10</v>
-      </c>
-      <c r="C25" t="s">
-        <v>149</v>
-      </c>
-      <c r="D25" t="s">
-        <v>150</v>
-      </c>
-      <c r="E25" t="s">
-        <v>151</v>
-      </c>
-      <c r="F25" t="s">
-        <v>14</v>
-      </c>
-      <c r="G25" t="s">
-        <v>14</v>
-      </c>
-      <c r="H25" t="s">
-        <v>14</v>
-      </c>
-      <c r="I25" t="s">
-        <v>14</v>
-      </c>
-      <c r="J25" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>